<commit_message>
update with 24 strokes characters
</commit_message>
<xml_diff>
--- a/Chinese Characters.xlsx
+++ b/Chinese Characters.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1731" uniqueCount="1278">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1756" uniqueCount="1294">
   <si>
     <t>Name</t>
   </si>
@@ -3845,6 +3845,54 @@
   </si>
   <si>
     <t>操守廉正而精明公正，中年成功隆昌而有官運與財運。</t>
+  </si>
+  <si>
+    <t>鑫</t>
+  </si>
+  <si>
+    <t>Handsome and talented, blessed with strong interpersonal harmony; enjoying honor and auspicious fortune, with favorable career or official luck.</t>
+  </si>
+  <si>
+    <t>英俊才人有人緣，榮貴吉祥而有官運。</t>
+  </si>
+  <si>
+    <t>豔</t>
+  </si>
+  <si>
+    <t>Refined, intelligent, and richly talented with a gentle disposition; enjoying auspicious fortune in midlife and flourishing prosperity in later years.</t>
+  </si>
+  <si>
+    <t>秀氣伶俐而多才賢淑，中年吉祥而晚年隆昌。</t>
+  </si>
+  <si>
+    <t>靈</t>
+  </si>
+  <si>
+    <t>Upright and principled, discerning clearly between righteousness and gain; astute and just, achieving success and prosperity in midlife with both fame and wealth.</t>
+  </si>
+  <si>
+    <t>義利分明而精明公正，中年成功隆昌而有名利。</t>
+  </si>
+  <si>
+    <t>靄</t>
+  </si>
+  <si>
+    <t>ǎi</t>
+  </si>
+  <si>
+    <t>Blessed with both fortune and prosperity, aided by benefactors; auspicious in midlife and flourishing abundantly in later years.</t>
+  </si>
+  <si>
+    <t>福祿雙收而貴人明現，中年吉祥而晚年隆昌。</t>
+  </si>
+  <si>
+    <t>靆</t>
+  </si>
+  <si>
+    <t>Refined and noble with abundant talents, possessing both wisdom and courage; attaining success and flourishing fortune in midlife.</t>
+  </si>
+  <si>
+    <t>清雅榮貴而多才，智勇雙全，中年成功隆昌。</t>
   </si>
 </sst>
 </file>
@@ -4134,7 +4182,7 @@
     <col customWidth="1" min="2" max="2" width="8.25"/>
     <col customWidth="1" min="3" max="3" width="7.88"/>
     <col customWidth="1" min="4" max="4" width="8.63"/>
-    <col customWidth="1" min="5" max="5" width="48.75"/>
+    <col customWidth="1" min="5" max="5" width="42.0"/>
     <col customWidth="1" min="6" max="6" width="39.63"/>
   </cols>
   <sheetData>
@@ -18325,12 +18373,24 @@
       <c r="AA346" s="3"/>
     </row>
     <row r="347">
-      <c r="A347" s="3"/>
-      <c r="B347" s="1"/>
-      <c r="C347" s="3"/>
-      <c r="D347" s="3"/>
-      <c r="E347" s="6"/>
-      <c r="F347" s="1"/>
+      <c r="A347" s="1" t="s">
+        <v>1278</v>
+      </c>
+      <c r="B347" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="C347" s="1">
+        <v>24.0</v>
+      </c>
+      <c r="D347" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E347" s="2" t="s">
+        <v>1279</v>
+      </c>
+      <c r="F347" s="1" t="s">
+        <v>1280</v>
+      </c>
       <c r="G347" s="3"/>
       <c r="H347" s="3"/>
       <c r="I347" s="3"/>
@@ -18354,12 +18414,24 @@
       <c r="AA347" s="3"/>
     </row>
     <row r="348">
-      <c r="A348" s="3"/>
-      <c r="B348" s="1"/>
-      <c r="C348" s="3"/>
-      <c r="D348" s="3"/>
-      <c r="E348" s="6"/>
-      <c r="F348" s="1"/>
+      <c r="A348" s="1" t="s">
+        <v>1281</v>
+      </c>
+      <c r="B348" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="C348" s="1">
+        <v>24.0</v>
+      </c>
+      <c r="D348" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E348" s="2" t="s">
+        <v>1282</v>
+      </c>
+      <c r="F348" s="1" t="s">
+        <v>1283</v>
+      </c>
       <c r="G348" s="3"/>
       <c r="H348" s="3"/>
       <c r="I348" s="3"/>
@@ -18383,12 +18455,24 @@
       <c r="AA348" s="3"/>
     </row>
     <row r="349">
-      <c r="A349" s="3"/>
-      <c r="B349" s="1"/>
-      <c r="C349" s="3"/>
-      <c r="D349" s="3"/>
-      <c r="E349" s="6"/>
-      <c r="F349" s="1"/>
+      <c r="A349" s="1" t="s">
+        <v>1284</v>
+      </c>
+      <c r="B349" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="C349" s="1">
+        <v>24.0</v>
+      </c>
+      <c r="D349" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E349" s="2" t="s">
+        <v>1285</v>
+      </c>
+      <c r="F349" s="1" t="s">
+        <v>1286</v>
+      </c>
       <c r="G349" s="3"/>
       <c r="H349" s="3"/>
       <c r="I349" s="3"/>
@@ -18412,12 +18496,24 @@
       <c r="AA349" s="3"/>
     </row>
     <row r="350">
-      <c r="A350" s="3"/>
-      <c r="B350" s="1"/>
-      <c r="C350" s="3"/>
-      <c r="D350" s="3"/>
-      <c r="E350" s="6"/>
-      <c r="F350" s="1"/>
+      <c r="A350" s="1" t="s">
+        <v>1287</v>
+      </c>
+      <c r="B350" s="1" t="s">
+        <v>1288</v>
+      </c>
+      <c r="C350" s="1">
+        <v>24.0</v>
+      </c>
+      <c r="D350" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E350" s="2" t="s">
+        <v>1289</v>
+      </c>
+      <c r="F350" s="1" t="s">
+        <v>1290</v>
+      </c>
       <c r="G350" s="3"/>
       <c r="H350" s="3"/>
       <c r="I350" s="3"/>
@@ -18441,12 +18537,24 @@
       <c r="AA350" s="3"/>
     </row>
     <row r="351">
-      <c r="A351" s="3"/>
-      <c r="B351" s="1"/>
-      <c r="C351" s="3"/>
-      <c r="D351" s="3"/>
-      <c r="E351" s="6"/>
-      <c r="F351" s="1"/>
+      <c r="A351" s="1" t="s">
+        <v>1291</v>
+      </c>
+      <c r="B351" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C351" s="1">
+        <v>24.0</v>
+      </c>
+      <c r="D351" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E351" s="2" t="s">
+        <v>1292</v>
+      </c>
+      <c r="F351" s="1" t="s">
+        <v>1293</v>
+      </c>
       <c r="G351" s="3"/>
       <c r="H351" s="3"/>
       <c r="I351" s="3"/>

</xml_diff>